<commit_message>
added exports of sch/brd files for both box and box-3 electronics
</commit_message>
<xml_diff>
--- a/ecad/bom.xlsx
+++ b/ecad/bom.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/esp-cpp/esp-box-emu/ecad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C81B13-A763-3647-9798-CB698B1A194E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA3D32A-FFDF-E744-B3B0-1A06B5FD05BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{FDF3D867-C8B7-C14D-9DEE-A50AF3FDFF6F}"/>
+    <workbookView xWindow="7960" yWindow="1140" windowWidth="34560" windowHeight="21580" xr2:uid="{FDF3D867-C8B7-C14D-9DEE-A50AF3FDFF6F}"/>
   </bookViews>
   <sheets>
-    <sheet name="esp-box-emu" sheetId="2" r:id="rId1"/>
+    <sheet name="esp-box-emu v2" sheetId="3" r:id="rId1"/>
+    <sheet name="esp-box-emu" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Electronics_Design_for_BOX_3_v2" localSheetId="0">'esp-box-emu v2'!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="136">
   <si>
     <t>Value</t>
   </si>
@@ -369,6 +373,81 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>HSMW-C170-U0000</t>
+  </si>
+  <si>
+    <t>LEDC2012X90N</t>
+  </si>
+  <si>
+    <t>BROADCOM LIMITED - HSMW-C170-U0000 - LED, WHITE, 670MCD, 0805</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Broadcom-Avago/HSMW-C170-U0000?qs=tMOYG%252Bw4%252BLwGyeHODzQdug%3D%3D</t>
+  </si>
+  <si>
+    <t>TL3340AF160QG</t>
+  </si>
+  <si>
+    <t>TL3340</t>
+  </si>
+  <si>
+    <t>S1, S2</t>
+  </si>
+  <si>
+    <t>E-SWITCH - TL3340AF160QG. - SWITCH, TACTILE SPST 50mA, SMD GULL WING</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/E-Switch/TL3340AF160QG?qs=Cv1v43EOJpo402rrfE5MlQ%3D%3D</t>
+  </si>
+  <si>
+    <t>AW9523BTQR</t>
+  </si>
+  <si>
+    <t>QFN50P400X400X80-25N</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>16 MULTI-FUNCTION LED DRIVER AND GPIO CONTROLLER WITH I2C INTERFACE</t>
+  </si>
+  <si>
+    <t>MCP73831/OT</t>
+  </si>
+  <si>
+    <t>SOT23-5L</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>MCP73831/2</t>
+  </si>
+  <si>
+    <t>MAX17048G+T1021-0168E_T822-3_MXM</t>
+  </si>
+  <si>
+    <t>21-0168E_T822-3_MXM</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>R12, R13, R27</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R20, R21, R22, R23, R24, R25, R26</t>
+  </si>
+  <si>
+    <t>C1, C3, C7</t>
   </si>
 </sst>
 </file>
@@ -435,6 +514,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{40617148-AC09-9344-9C2F-51E038337952}" name="Table13" displayName="Table13" ref="A1:H24" totalsRowShown="0">
+  <autoFilter ref="A1:H24" xr:uid="{40617148-AC09-9344-9C2F-51E038337952}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{30D1DAB2-B750-E546-838E-EC140FCE2F48}" name="Qty"/>
+    <tableColumn id="2" xr3:uid="{E04CEEE8-3C91-4B4E-9F03-75190A1D9BE8}" name="Value"/>
+    <tableColumn id="3" xr3:uid="{B0E27E87-CE9D-F348-A677-A6024611D247}" name="Device"/>
+    <tableColumn id="4" xr3:uid="{994CBA8C-8196-E543-B06B-74C499B97359}" name="Package"/>
+    <tableColumn id="5" xr3:uid="{77B9E742-5928-D84A-A7FD-D38553861CAB}" name="Parts"/>
+    <tableColumn id="6" xr3:uid="{3B0E23AA-B40F-5F45-8507-203A389FBA30}" name="Description"/>
+    <tableColumn id="7" xr3:uid="{02B82134-160C-C047-BA8D-17209E59CC5E}" name="Order Link"/>
+    <tableColumn id="8" xr3:uid="{C98C5DA6-4187-704C-810E-5F41E0767462}" name="Alternate"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BB277A32-B838-834E-9B90-8C32D17655D8}" name="Table1" displayName="Table1" ref="A1:H24" totalsRowShown="0">
   <autoFilter ref="A1:H24" xr:uid="{BB277A32-B838-834E-9B90-8C32D17655D8}"/>
   <tableColumns count="8">
@@ -747,11 +843,696 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DC11FC-E987-E64E-A1F4-3F37FD4F3BB6}">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="67.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="10" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>629722000214</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F16" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" t="s">
+        <v>127</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G22" r:id="rId1" display="https://www.mouser.com/ProductDetail/649-67996-112HLF" xr:uid="{F93D408C-948D-E642-AD8A-2555542E870F}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{8F3AD5E7-38BE-8D45-9463-E9609A5D0F6F}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{96E67669-A4D7-844C-896B-90B4B6A3346D}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{379A4D82-FBE8-7C42-A6A6-9130E4D868D3}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{9563E78E-2F67-F44A-9A73-C3F63CC21863}"/>
+    <hyperlink ref="G6" r:id="rId6" xr:uid="{BB8075EE-E4AB-5D41-B0FC-AFE117891286}"/>
+    <hyperlink ref="G7" r:id="rId7" xr:uid="{68B92F17-6E10-CC46-BA5C-14022AB2C9B4}"/>
+    <hyperlink ref="G8" r:id="rId8" xr:uid="{3A403D01-04FF-D747-A1D2-DB938AEEB3BF}"/>
+    <hyperlink ref="G9" r:id="rId9" xr:uid="{634B11B8-1F01-FB41-BCE9-6CA6D7DD43E8}"/>
+    <hyperlink ref="G10" r:id="rId10" xr:uid="{5406B994-FE92-DD49-9719-11640783ABC4}"/>
+    <hyperlink ref="G11" r:id="rId11" xr:uid="{9A456B11-1DBB-4441-8D10-3A338B74A364}"/>
+    <hyperlink ref="G12" r:id="rId12" xr:uid="{847B50D4-0044-8443-A5B5-F9A9C11A63E1}"/>
+    <hyperlink ref="G13" r:id="rId13" xr:uid="{C2C3CC04-790B-3E4E-83A4-FE45D5170516}"/>
+    <hyperlink ref="G15" r:id="rId14" xr:uid="{6195EC73-89F0-0B40-8DA6-CAEF25799D2B}"/>
+    <hyperlink ref="G17" r:id="rId15" xr:uid="{70E1F5DD-D364-CE4F-9F9C-5D71C616276D}"/>
+    <hyperlink ref="G20" r:id="rId16" xr:uid="{79F27EAD-81DD-534D-8FF5-2A9F088F491D}"/>
+    <hyperlink ref="G21" r:id="rId17" xr:uid="{3AD4239C-5607-484C-8590-4BC2E854A736}"/>
+    <hyperlink ref="G24" r:id="rId18" xr:uid="{87D0F851-664E-494C-ACE4-C16C0E8E3A9D}"/>
+    <hyperlink ref="H22" r:id="rId19" xr:uid="{5D017E52-5A95-0249-814B-C77C0F4B6ED0}"/>
+    <hyperlink ref="G14" r:id="rId20" xr:uid="{F2247098-6999-4642-9F79-12D43E5BB422}"/>
+    <hyperlink ref="G23" r:id="rId21" xr:uid="{5C5A1499-A99D-BF43-A967-36551157F18C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId22"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3445F7F-1D76-0F48-982D-8E2CE0A72BAE}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>